<commit_message>
Fixing this month balance problem, more advance copy function.
</commit_message>
<xml_diff>
--- a/WebContent/template/template.xlsx
+++ b/WebContent/template/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>EMSTF Resident Support &amp; Computer Operation Support Services Team Roster</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t>No. of working day</t>
-  </si>
-  <si>
-    <t>h</t>
   </si>
   <si>
     <t>Vacant Shifts</t>
@@ -845,7 +842,7 @@
   <dimension ref="A1:AQ18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -859,11 +856,12 @@
     <col min="35" max="35" width="8.25" customWidth="1"/>
     <col min="36" max="36" width="8.625" customWidth="1"/>
     <col min="37" max="37" width="7.875" customWidth="1"/>
-    <col min="38" max="38" width="4.5" customWidth="1"/>
-    <col min="39" max="39" width="5.625" customWidth="1"/>
-    <col min="40" max="41" width="4.5" customWidth="1"/>
-    <col min="42" max="42" width="3.375" customWidth="1"/>
-    <col min="43" max="43" width="6.25" customWidth="1"/>
+    <col min="38" max="38" width="4.5" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="5.625" hidden="1" customWidth="1"/>
+    <col min="40" max="41" width="4.5" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="3.375" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="6.25" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="19.5">
@@ -1127,7 +1125,7 @@
     </row>
     <row r="7" spans="1:43">
       <c r="A7" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -1159,9 +1157,6 @@
       <c r="AC7" s="10"/>
       <c r="AD7" s="10"/>
       <c r="AE7" s="10"/>
-      <c r="AF7" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="8" spans="1:43" ht="18.75">
       <c r="A8" s="11" t="s">

</xml_diff>

<commit_message>
Fix the last vacant cell style problem
</commit_message>
<xml_diff>
--- a/WebContent/template/template.xlsx
+++ b/WebContent/template/template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="4200" windowWidth="28035" windowHeight="12345"/>
+    <workbookView xWindow="2076" yWindow="4200" windowWidth="23256" windowHeight="12348"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,13 +179,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\+#0.##;\-#0.##"/>
+    <numFmt numFmtId="176" formatCode="\+#0.##;\-#0.##"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -225,7 +225,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -248,6 +248,13 @@
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -406,7 +413,7 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -842,29 +849,29 @@
   <dimension ref="A1:AQ18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH12" sqref="AH12"/>
+      <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="25.625" customWidth="1"/>
-    <col min="2" max="21" width="3.125" customWidth="1"/>
-    <col min="22" max="22" width="2.875" customWidth="1"/>
-    <col min="23" max="32" width="3.125" customWidth="1"/>
-    <col min="33" max="33" width="10.125" customWidth="1"/>
-    <col min="34" max="34" width="8.875" customWidth="1"/>
-    <col min="35" max="35" width="8.25" customWidth="1"/>
-    <col min="36" max="36" width="8.625" customWidth="1"/>
-    <col min="37" max="37" width="7.875" customWidth="1"/>
-    <col min="38" max="38" width="4.5" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="5.625" hidden="1" customWidth="1"/>
-    <col min="40" max="41" width="4.5" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="3.375" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="6.25" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="21" width="3.109375" customWidth="1"/>
+    <col min="22" max="22" width="2.88671875" customWidth="1"/>
+    <col min="23" max="32" width="3.109375" customWidth="1"/>
+    <col min="33" max="33" width="10.109375" customWidth="1"/>
+    <col min="34" max="34" width="8.88671875" customWidth="1"/>
+    <col min="35" max="35" width="8.21875" customWidth="1"/>
+    <col min="36" max="36" width="8.6640625" customWidth="1"/>
+    <col min="37" max="37" width="7.88671875" customWidth="1"/>
+    <col min="38" max="38" width="4.44140625" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="5.6640625" hidden="1" customWidth="1"/>
+    <col min="40" max="41" width="4.44140625" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="3.33203125" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="6.21875" hidden="1" customWidth="1"/>
     <col min="44" max="44" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="19.5">
+    <row r="1" spans="1:43" ht="19.8">
       <c r="A1" s="2"/>
       <c r="B1" s="32" t="s">
         <v>0</v>
@@ -911,7 +918,7 @@
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:43" ht="18.75">
+    <row r="2" spans="1:43" ht="17.399999999999999">
       <c r="A2" s="1"/>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
@@ -1058,7 +1065,7 @@
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
     </row>
-    <row r="6" spans="1:43" ht="31.5">
+    <row r="6" spans="1:43" ht="31.2">
       <c r="A6" s="22" t="s">
         <v>40</v>
       </c>
@@ -1157,8 +1164,9 @@
       <c r="AC7" s="10"/>
       <c r="AD7" s="10"/>
       <c r="AE7" s="10"/>
-    </row>
-    <row r="8" spans="1:43" ht="18.75">
+      <c r="AF7" s="10"/>
+    </row>
+    <row r="8" spans="1:43" ht="18">
       <c r="A8" s="11" t="s">
         <v>2</v>
       </c>
@@ -1192,7 +1200,7 @@
       <c r="AA8" s="31"/>
       <c r="AB8" s="31"/>
     </row>
-    <row r="9" spans="1:43" ht="18.75">
+    <row r="9" spans="1:43" ht="18">
       <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
@@ -1226,7 +1234,7 @@
       <c r="AA9" s="31"/>
       <c r="AB9" s="31"/>
     </row>
-    <row r="10" spans="1:43" ht="18.75">
+    <row r="10" spans="1:43" ht="18">
       <c r="A10" s="13" t="s">
         <v>6</v>
       </c>
@@ -1258,7 +1266,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:43" ht="18.75">
+    <row r="11" spans="1:43" ht="18">
       <c r="A11" s="14" t="s">
         <v>7</v>
       </c>
@@ -1296,7 +1304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:43" ht="18.75">
+    <row r="12" spans="1:43" ht="18">
       <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
@@ -1332,7 +1340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:43" ht="18.75">
+    <row r="13" spans="1:43" ht="18">
       <c r="A13" s="16" t="s">
         <v>14</v>
       </c>
@@ -1368,7 +1376,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:43" ht="18.75">
+    <row r="14" spans="1:43" ht="18">
       <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
@@ -1404,7 +1412,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:43" ht="18.75">
+    <row r="15" spans="1:43" ht="18">
       <c r="A15" s="16" t="s">
         <v>20</v>
       </c>
@@ -1436,7 +1444,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:43" ht="18.75">
+    <row r="16" spans="1:43" ht="18">
       <c r="A16" s="18" t="s">
         <v>21</v>
       </c>
@@ -1468,7 +1476,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" ht="18.75">
+    <row r="17" spans="1:28" ht="18">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -1543,6 +1551,7 @@
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="B2:AF2"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -1556,7 +1565,7 @@
       <selection activeCell="N13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <sheetData>
     <row r="1" spans="1:43">
       <c r="A1" t="s">
@@ -1618,7 +1627,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:43" ht="18.75">
+    <row r="13" spans="1:43" ht="18">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1691,6 +1700,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="B13:AF13">
     <cfRule type="cellIs" dxfId="3" priority="104" operator="equal">
       <formula>"c"</formula>
@@ -1716,8 +1726,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <sheetData/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>